<commit_message>
Update M40 numbers for GEMM fix
</commit_message>
<xml_diff>
--- a/results/DeepBench_NV_M40.xlsx
+++ b/results/DeepBench_NV_M40.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27430"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="16900" tabRatio="500"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="29780" windowHeight="18380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -700,7 +700,7 @@
   <dimension ref="A1:AC207"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="A197" sqref="A197:XFD197"/>
+      <selection activeCell="A74" sqref="A74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2077,11 +2077,11 @@
         <v>10</v>
       </c>
       <c r="I56" s="2">
-        <v>64.221000000000004</v>
+        <v>46.712000000000003</v>
       </c>
       <c r="J56" s="2">
         <f t="shared" si="0"/>
-        <v>2.5624771261736816</v>
+        <v>3.5229671930125019</v>
       </c>
       <c r="K56" s="2"/>
     </row>
@@ -2102,11 +2102,11 @@
         <v>10</v>
       </c>
       <c r="I57" s="2">
-        <v>0.70299999999999996</v>
+        <v>0.68500000000000005</v>
       </c>
       <c r="J57" s="2">
         <f t="shared" si="0"/>
-        <v>1.482080227596017</v>
+        <v>1.5210254014598537</v>
       </c>
       <c r="K57" s="2"/>
     </row>
@@ -2127,11 +2127,11 @@
         <v>10</v>
       </c>
       <c r="I58" s="2">
-        <v>56.040999999999997</v>
+        <v>53.628</v>
       </c>
       <c r="J58" s="2">
         <f t="shared" si="0"/>
-        <v>3.4170274637497551</v>
+        <v>3.5707771331394049</v>
       </c>
       <c r="K58" s="2"/>
     </row>
@@ -2152,11 +2152,11 @@
         <v>10</v>
       </c>
       <c r="I59" s="2">
-        <v>0.68899999999999995</v>
+        <v>0.79</v>
       </c>
       <c r="J59" s="2">
         <f t="shared" si="0"/>
-        <v>1.7596451669085633</v>
+        <v>1.5346778734177213</v>
       </c>
       <c r="K59" s="2"/>
     </row>
@@ -2177,11 +2177,11 @@
         <v>10</v>
       </c>
       <c r="I60" s="2">
-        <v>78.483999999999995</v>
+        <v>71.004999999999995</v>
       </c>
       <c r="J60" s="2">
         <f t="shared" si="0"/>
-        <v>3.049883353549768</v>
+        <v>3.3711294291951268</v>
       </c>
       <c r="K60" s="2"/>
     </row>
@@ -2202,11 +2202,11 @@
         <v>10</v>
       </c>
       <c r="I61" s="2">
-        <v>0.86199999999999999</v>
+        <v>0.97799999999999998</v>
       </c>
       <c r="J61" s="2">
         <f t="shared" si="0"/>
-        <v>1.7581141531322504</v>
+        <v>1.54958527607362</v>
       </c>
       <c r="K61" s="2"/>
     </row>
@@ -2227,11 +2227,11 @@
         <v>10</v>
       </c>
       <c r="I62" s="2">
-        <v>122.86499999999999</v>
+        <v>110.792</v>
       </c>
       <c r="J62" s="2">
         <f t="shared" si="0"/>
-        <v>3.1171389101208646</v>
+        <v>3.4568134178641055</v>
       </c>
       <c r="K62" s="2"/>
     </row>
@@ -2252,11 +2252,11 @@
         <v>10</v>
       </c>
       <c r="I63" s="2">
-        <v>1.4019999999999999</v>
+        <v>1.5409999999999999</v>
       </c>
       <c r="J63" s="2">
         <f t="shared" si="0"/>
-        <v>1.7295228530670474</v>
+        <v>1.5735178715120053</v>
       </c>
       <c r="K63" s="2"/>
     </row>
@@ -2382,11 +2382,11 @@
         <v>10</v>
       </c>
       <c r="I69" s="2">
-        <v>0.89600000000000002</v>
+        <v>0.90100000000000002</v>
       </c>
       <c r="J69" s="2">
         <f t="shared" si="1"/>
-        <v>0.70217142857142856</v>
+        <v>0.69827480577136514</v>
       </c>
       <c r="K69" s="2"/>
     </row>
@@ -2407,11 +2407,11 @@
         <v>10</v>
       </c>
       <c r="I70" s="2">
-        <v>0.89200000000000002</v>
+        <v>0.90700000000000003</v>
       </c>
       <c r="J70" s="2">
         <f t="shared" si="1"/>
-        <v>1.4106403587443945</v>
+        <v>1.3873111356119072</v>
       </c>
       <c r="K70" s="2"/>
     </row>
@@ -2432,11 +2432,11 @@
         <v>10</v>
       </c>
       <c r="I71" s="2">
-        <v>1.5129999999999999</v>
+        <v>1.1619999999999999</v>
       </c>
       <c r="J71" s="2">
         <f t="shared" si="1"/>
-        <v>1.6633062789160611</v>
+        <v>2.1657335628227199</v>
       </c>
       <c r="K71" s="2"/>
     </row>
@@ -2457,11 +2457,11 @@
         <v>10</v>
       </c>
       <c r="I72" s="2">
-        <v>1.766</v>
+        <v>1.885</v>
       </c>
       <c r="J72" s="2">
         <f t="shared" si="1"/>
-        <v>2.8500366930917331</v>
+        <v>2.670113952254642</v>
       </c>
       <c r="K72" s="2"/>
     </row>
@@ -2587,11 +2587,11 @@
         <v>10</v>
       </c>
       <c r="I77" s="2">
-        <v>0.159</v>
+        <v>0.23100000000000001</v>
       </c>
       <c r="J77" s="2">
         <f t="shared" si="1"/>
-        <v>0.63310249056603773</v>
+        <v>0.43577184415584419</v>
       </c>
       <c r="K77" s="2"/>
     </row>
@@ -2613,11 +2613,11 @@
         <v>10</v>
       </c>
       <c r="I78" s="2">
-        <v>0.16</v>
+        <v>0.23200000000000001</v>
       </c>
       <c r="J78" s="2">
         <f t="shared" si="1"/>
-        <v>1.2582911999999999</v>
+        <v>0.86778703448275862</v>
       </c>
       <c r="K78" s="2"/>
     </row>
@@ -2639,11 +2639,11 @@
         <v>10</v>
       </c>
       <c r="I79" s="2">
-        <v>0.39</v>
+        <v>0.254</v>
       </c>
       <c r="J79" s="2">
         <f t="shared" si="1"/>
-        <v>1.0324440615384616</v>
+        <v>1.585248755905512</v>
       </c>
       <c r="K79" s="2"/>
     </row>
@@ -2665,11 +2665,11 @@
         <v>10</v>
       </c>
       <c r="I80" s="2">
-        <v>0.53800000000000003</v>
+        <v>0.22600000000000001</v>
       </c>
       <c r="J80" s="2">
         <f t="shared" si="1"/>
-        <v>1.4968519851301114</v>
+        <v>3.5633025132743361</v>
       </c>
       <c r="K80" s="2"/>
     </row>

</xml_diff>